<commit_message>
Additional Fields in Audit Report
</commit_message>
<xml_diff>
--- a/App_Templates/TABill_Template.xlsx
+++ b/App_Templates/TABill_Template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\WebTA1\App_Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5533F134-5D94-4DB0-B74A-4C8072D9F262}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>TA Bill Date</t>
   </si>
@@ -120,12 +126,30 @@
   <si>
     <t>Passed 
 Amount</t>
+  </si>
+  <si>
+    <t>Emp. Category</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Cost Center</t>
+  </si>
+  <si>
+    <t>VCH No</t>
+  </si>
+  <si>
+    <t>VCH Date</t>
+  </si>
+  <si>
+    <t>VCH Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -180,11 +204,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -203,9 +264,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -217,6 +287,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -265,7 +338,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -298,9 +371,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,6 +423,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -508,104 +615,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:BJ7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" customWidth="1"/>
-    <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.5703125" customWidth="1"/>
-    <col min="31" max="31" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
+    <col min="6" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="18" width="10.140625" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.7109375" customWidth="1"/>
+    <col min="29" max="29" width="9.85546875" customWidth="1"/>
+    <col min="30" max="30" width="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.42578125" customWidth="1"/>
-    <col min="37" max="37" width="6.7109375" customWidth="1"/>
-    <col min="38" max="38" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.85546875" customWidth="1"/>
-    <col min="43" max="43" width="6.5703125" customWidth="1"/>
-    <col min="44" max="44" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.140625" customWidth="1"/>
-    <col min="49" max="49" width="6.7109375" customWidth="1"/>
-    <col min="50" max="50" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.140625" customWidth="1"/>
+    <col min="33" max="33" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.5703125" customWidth="1"/>
+    <col min="39" max="39" width="6.28515625" customWidth="1"/>
+    <col min="40" max="40" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.42578125" customWidth="1"/>
+    <col min="45" max="45" width="6.7109375" customWidth="1"/>
+    <col min="46" max="46" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.85546875" customWidth="1"/>
+    <col min="51" max="51" width="6.5703125" customWidth="1"/>
+    <col min="52" max="52" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.140625" customWidth="1"/>
+    <col min="57" max="57" width="6.7109375" customWidth="1"/>
+    <col min="58" max="58" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:62" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="N1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
       <c r="W1" s="7"/>
       <c r="X1" s="7"/>
       <c r="Y1" s="7"/>
@@ -613,307 +735,341 @@
       <c r="AA1" s="7"/>
       <c r="AB1" s="7"/>
       <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7" t="s">
+      <c r="AD1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7" t="s">
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AL1" s="7"/>
-      <c r="AM1" s="7"/>
-      <c r="AN1" s="7"/>
-      <c r="AO1" s="7"/>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="7" t="s">
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AR1" s="7"/>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="7"/>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7" t="s">
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
     </row>
-    <row r="2" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8" t="s">
+    <row r="2" spans="1:62" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8" t="s">
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8" t="s">
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="AA2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="AB2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="AC2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="AD2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="AE2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="AF2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8" t="s">
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8" t="s">
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AK2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AL2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AM2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AN2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AO2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AP2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AQ2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AR2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AS2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="8" t="s">
+      <c r="AT2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AM2" s="8" t="s">
+      <c r="AU2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AN2" s="8" t="s">
+      <c r="AV2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AW2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AP2" s="8" t="s">
+      <c r="AX2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AQ2" s="8" t="s">
+      <c r="AY2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AR2" s="8" t="s">
+      <c r="AZ2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AS2" s="8" t="s">
+      <c r="BA2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AT2" s="8" t="s">
+      <c r="BB2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AU2" s="8" t="s">
+      <c r="BC2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AV2" s="8" t="s">
+      <c r="BD2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AW2" s="8" t="s">
+      <c r="BE2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AX2" s="8" t="s">
+      <c r="BF2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AY2" s="8" t="s">
+      <c r="BG2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AZ2" s="8" t="s">
+      <c r="BH2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BA2" s="8" t="s">
+      <c r="BI2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="BB2" s="8" t="s">
+      <c r="BJ2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="3" t="s">
+    <row r="3" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="4" t="s">
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="AH3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AI3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="8"/>
-      <c r="AK3" s="8"/>
-      <c r="AL3" s="8"/>
-      <c r="AM3" s="8"/>
-      <c r="AN3" s="8"/>
-      <c r="AO3" s="8"/>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="8"/>
-      <c r="AT3" s="8"/>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="8"/>
-      <c r="AX3" s="8"/>
-      <c r="AY3" s="8"/>
-      <c r="AZ3" s="8"/>
-      <c r="BA3" s="8"/>
-      <c r="BB3" s="8"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7"/>
+      <c r="AL3" s="7"/>
+      <c r="AM3" s="7"/>
+      <c r="AN3" s="7"/>
+      <c r="AO3" s="7"/>
+      <c r="AP3" s="7"/>
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="7"/>
+      <c r="AT3" s="7"/>
+      <c r="AU3" s="7"/>
+      <c r="AV3" s="7"/>
+      <c r="AW3" s="7"/>
+      <c r="AX3" s="7"/>
+      <c r="AY3" s="7"/>
+      <c r="AZ3" s="7"/>
+      <c r="BA3" s="7"/>
+      <c r="BB3" s="7"/>
+      <c r="BC3" s="7"/>
+      <c r="BD3" s="7"/>
+      <c r="BE3" s="7"/>
+      <c r="BF3" s="7"/>
+      <c r="BG3" s="7"/>
+      <c r="BH3" s="7"/>
+      <c r="BI3" s="7"/>
+      <c r="BJ3" s="7"/>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="K1:U1"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="V1:AD1"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AE1:AJ1"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="AQ1:AV1"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AR2:AR3"/>
+  <mergeCells count="62">
+    <mergeCell ref="BE1:BJ1"/>
+    <mergeCell ref="BE2:BE3"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="BI2:BI3"/>
+    <mergeCell ref="BJ2:BJ3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY1:BD1"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="AS1:AX1"/>
     <mergeCell ref="AS2:AS3"/>
     <mergeCell ref="AT2:AT3"/>
     <mergeCell ref="AU2:AU3"/>
     <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AK1:AP1"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AM1:AR1"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AJ2:AJ3"/>
     <mergeCell ref="AK2:AK3"/>
     <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AW1:BB1"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="AD1:AL1"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="S1:AC1"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>